<commit_message>
Moduly 36 a 37 (z krouzku) pojmenovany.
Upraveny nazvy ve vykresech. Pocatky presunuty do [0;0].
</commit_message>
<xml_diff>
--- a/TT-moduly.xlsx
+++ b/TT-moduly.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UsersData\vlak\AutoCad\Bloky\TT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vladimír\Downloads\tt-moduly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18075" windowHeight="9975"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="18075" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SeznamModulu" sheetId="1" r:id="rId1"/>
@@ -198,12 +198,6 @@
     <t>nedokončeno</t>
   </si>
   <si>
-    <t>Kroužek 13/14</t>
-  </si>
-  <si>
-    <t>Kroužek 13/14 II</t>
-  </si>
-  <si>
     <t>Aktualizace: 16. 7. 2017</t>
   </si>
   <si>
@@ -223,12 +217,18 @@
   </si>
   <si>
     <t>Čejč východ</t>
+  </si>
+  <si>
+    <t>Bunkr (kroužek 13/14)</t>
+  </si>
+  <si>
+    <t>Tábor (kroužek 16/17)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,47 +603,47 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -778,14 +778,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabulka1" displayName="Tabulka1" ref="A3:E53" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabulka1" displayName="Tabulka1" ref="A3:E53" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A3:E53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" name="Název" dataDxfId="3"/>
-    <tableColumn id="3" name="Začátek výroby" dataDxfId="2"/>
-    <tableColumn id="4" name="Konec výroby" dataDxfId="1"/>
-    <tableColumn id="5" name="Verze zapojení" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Název" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Začátek výroby" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Konec výroby" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Verze zapojení" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -794,7 +794,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -832,7 +832,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -867,6 +867,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -902,9 +919,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1077,12 +1111,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,13 +1127,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
@@ -1559,54 +1593,54 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="42" t="s">
+      <c r="C36" s="37"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="42" t="s">
+      <c r="C37" s="37"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="41" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="42" t="s">
+      <c r="C38" s="37"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="42" t="s">
+      <c r="C39" s="37"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1656,28 +1690,28 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="36">
+      <c r="A43" s="35">
         <v>34</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="39" t="s">
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="38" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="40">
+      <c r="A44" s="39">
         <v>35</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="38"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="42" t="s">
+      <c r="C44" s="37"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="41" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1686,7 +1720,7 @@
         <v>36</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C45" s="19">
         <v>41518</v>
@@ -1701,38 +1735,40 @@
         <v>37</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="26"/>
+        <v>66</v>
+      </c>
+      <c r="C46" s="26">
+        <v>42614</v>
+      </c>
       <c r="D46" s="27"/>
       <c r="E46" s="28" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="40">
+      <c r="A47" s="39">
         <v>38</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="42"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="41"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="40">
+      <c r="A48" s="39">
         <v>39</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="42"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="41"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C49" s="26"/>
       <c r="D49" s="27"/>
@@ -1742,10 +1778,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="27"/>
@@ -1755,10 +1791,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
@@ -1767,13 +1803,13 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="40">
+      <c r="A52" s="39">
         <v>41</v>
       </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="42"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="41"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
@@ -1785,15 +1821,15 @@
       <c r="E53" s="15"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="48"/>
+      <c r="A54" s="44"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="47"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Odstranit stare nazvy modulu uplne (krouzek xy).
</commit_message>
<xml_diff>
--- a/TT-moduly.xlsx
+++ b/TT-moduly.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vladimír\Downloads\tt-moduly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UsersData\vlak\AutoCad\Bloky\TT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18075" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="18075" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="SeznamModulu" sheetId="1" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t>nedokončeno</t>
   </si>
   <si>
-    <t>Aktualizace: 16. 7. 2017</t>
-  </si>
-  <si>
     <t>40a</t>
   </si>
   <si>
@@ -219,16 +216,19 @@
     <t>Čejč východ</t>
   </si>
   <si>
-    <t>Bunkr (kroužek 13/14)</t>
-  </si>
-  <si>
-    <t>Tábor (kroužek 16/17)</t>
+    <t>Bunkr</t>
+  </si>
+  <si>
+    <t>Tábor</t>
+  </si>
+  <si>
+    <t>Aktualizace: 16. 10. 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -778,14 +778,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabulka1" displayName="Tabulka1" ref="A3:E53" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabulka1" displayName="Tabulka1" ref="A3:E53" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A3:E53"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Název" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Začátek výroby" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Konec výroby" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Verze zapojení" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" name="Název" dataDxfId="3"/>
+    <tableColumn id="3" name="Začátek výroby" dataDxfId="2"/>
+    <tableColumn id="4" name="Konec výroby" dataDxfId="1"/>
+    <tableColumn id="5" name="Verze zapojení" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -794,7 +794,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kancelář">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -832,7 +832,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kancelář">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -867,23 +867,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -919,26 +902,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kancelář">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1111,12 +1077,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,7 +1686,7 @@
         <v>36</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="19">
         <v>41518</v>
@@ -1735,7 +1701,7 @@
         <v>37</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" s="26">
         <v>42614</v>
@@ -1765,10 +1731,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C49" s="26"/>
       <c r="D49" s="27"/>
@@ -1778,10 +1744,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="26"/>
       <c r="D50" s="27"/>
@@ -1791,10 +1757,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
@@ -1829,7 +1795,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Doplnit zbyle moduly Cejc.
</commit_message>
<xml_diff>
--- a/TT-moduly.xlsx
+++ b/TT-moduly.xlsx
@@ -15,14 +15,14 @@
     <sheet name="SeznamModulu" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SeznamModulu!$A$3:$E$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SeznamModulu!$A$3:$E$56</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
   <si>
     <t>Modul s kobercem</t>
   </si>
@@ -222,7 +222,19 @@
     <t>Tábor</t>
   </si>
   <si>
-    <t>Aktualizace: 16. 10. 2017</t>
+    <t>Aktualizace: 16. 12. 2018</t>
+  </si>
+  <si>
+    <t>40d</t>
+  </si>
+  <si>
+    <t>Čejč DK</t>
+  </si>
+  <si>
+    <t>Čejč sudý vjezd</t>
+  </si>
+  <si>
+    <t>Čejč lichý vjezd</t>
   </si>
 </sst>
 </file>
@@ -778,8 +790,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabulka1" displayName="Tabulka1" ref="A3:E53" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="A3:E53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabulka1" displayName="Tabulka1" ref="A3:E56" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A3:E56"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID" dataDxfId="4"/>
     <tableColumn id="2" name="Název" dataDxfId="3"/>
@@ -1078,11 +1090,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,8 +1230,8 @@
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="10">
-        <v>1</v>
+      <c r="E11" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1257,8 +1269,8 @@
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
-      <c r="E14" s="10">
-        <v>1</v>
+      <c r="E14" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1379,8 +1391,8 @@
       <c r="D22" s="20">
         <v>40483</v>
       </c>
-      <c r="E22" s="10">
-        <v>1</v>
+      <c r="E22" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1697,17 +1709,19 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="24">
+      <c r="A46" s="39">
         <v>37</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="26">
+      <c r="C46" s="37">
         <v>42614</v>
       </c>
-      <c r="D46" s="27"/>
-      <c r="E46" s="28" t="s">
+      <c r="D46" s="40">
+        <v>43101</v>
+      </c>
+      <c r="E46" s="41" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1760,46 +1774,79 @@
         <v>60</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
-      <c r="E51" s="28" t="s">
-        <v>25</v>
-      </c>
+      <c r="E51" s="28"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="39">
+      <c r="A52" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="26"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="24">
         <v>41</v>
       </c>
-      <c r="B52" s="36"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="41"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="8">
+      <c r="B53" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="26"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="28"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="24">
         <v>42</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="15"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="47"/>
+      <c r="B54" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="26"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="28"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="39">
+        <v>43</v>
+      </c>
+      <c r="B55" s="36"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="41"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
+        <v>44</v>
+      </c>
+      <c r="B56" s="18"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="15"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="44"/>
+      <c r="B57" s="45"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="47"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="29" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="29" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pridat moduly krouzek 2018/2019.
</commit_message>
<xml_diff>
--- a/TT-moduly.xlsx
+++ b/TT-moduly.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Modul s kobercem</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>Čejč lichý vjezd</t>
+  </si>
+  <si>
+    <t>Kroužek 2018/2019 I</t>
+  </si>
+  <si>
+    <t>Kroužek 2018/2019 II</t>
   </si>
 </sst>
 </file>
@@ -1093,8 +1099,8 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,8 +1735,12 @@
       <c r="A47" s="39">
         <v>38</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="37"/>
+      <c r="B47" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="37">
+        <v>43344</v>
+      </c>
       <c r="D47" s="40"/>
       <c r="E47" s="41"/>
     </row>
@@ -1738,8 +1748,12 @@
       <c r="A48" s="39">
         <v>39</v>
       </c>
-      <c r="B48" s="36"/>
-      <c r="C48" s="37"/>
+      <c r="B48" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="37">
+        <v>43344</v>
+      </c>
       <c r="D48" s="40"/>
       <c r="E48" s="41"/>
     </row>

</xml_diff>